<commit_message>
feat: being more specific in explaining the usage of excel file.
</commit_message>
<xml_diff>
--- a/update/metrics_excel.xlsx
+++ b/update/metrics_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\python\Automated-Telemetry-Monitor\update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D4BBBB-D29E-4256-A97C-11C9ADC206A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62481C23-03E5-4E5E-A67A-7B78C397348A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="454">
   <si>
     <t>Enabled</t>
   </si>
@@ -144,156 +144,12 @@
     <t>N</t>
   </si>
   <si>
-    <t>CPU Busy</t>
-  </si>
-  <si>
-    <t>100 * (1 - avg(rate(node_cpu_seconds_total{mode=\"idle\", instance=\"$node\"}[$__rate_interval])))</t>
-  </si>
-  <si>
-    <t>System Load</t>
-  </si>
-  <si>
-    <t>node_load1{instance="$hostname:9100"}</t>
-  </si>
-  <si>
     <t>1minute</t>
   </si>
   <si>
-    <t>RAM Used</t>
-  </si>
-  <si>
-    <t>(1 - (node_memory_MemAvailable_bytes{instance=\"$node\", job=\"$job\"} / node_memory_MemTotal_bytes{instance=\"$node\", job=\"$job\"})) * 100</t>
-  </si>
-  <si>
-    <t>System Memory Usage</t>
-  </si>
-  <si>
-    <t>Used Current</t>
-  </si>
-  <si>
-    <t>node_memory_MemTotal_bytes{instance="$hostname:9100"} - node_memory_MemFree_bytes{instance="$hostname:9100"} - node_memory_Buffers_bytes{instance="$hostname:9100"} - node_memory_Cached_bytes{instance="$hostname:9100"}</t>
-  </si>
-  <si>
-    <t>Free Current</t>
-  </si>
-  <si>
-    <t>node_memory_MemFree_bytes{instance="$hostname:9100"}</t>
-  </si>
-  <si>
-    <t>Memory Usage</t>
-  </si>
-  <si>
-    <t>((node_memory_MemTotal_bytes{instance="$hostname:9100"} - node_memory_MemFree_bytes{instance="$hostname:9100"} - node_memory_Buffers_bytes{instance="$hostname:9100"} - node_memory_Cached_bytes{instance="$hostname:9100"}) / node_memory_MemTotal_bytes{instance="$hostname:9100"}) * 100</t>
-  </si>
-  <si>
-    <t>PCIe Throughput</t>
-  </si>
-  <si>
-    <t>Tx Current</t>
-  </si>
-  <si>
-    <t>sum(DCGM_FI_PROF_PCIE_TX_BYTES{instance=\"$hostname:9400\"})</t>
-  </si>
-  <si>
-    <t>Rx Current</t>
-  </si>
-  <si>
-    <t>sum(DCGM_FI_PROF_PCIE_RX_BYTES{instance=\"$hostname:9400\"})</t>
-  </si>
-  <si>
-    <t>Network Metrics</t>
-  </si>
-  <si>
-    <t>NVLINK Bandwidth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Current </t>
-  </si>
-  <si>
-    <t>1e6*sum(DCGM_FI_DEV_NVLINK_BANDWIDTH_TOTAL{instance="hgx3b:9400"})</t>
-  </si>
-  <si>
-    <t>Ethernet Throughput</t>
-  </si>
-  <si>
-    <t>Transmit Current</t>
-  </si>
-  <si>
-    <t>sum(rate(node_network_transmit_bytes_total{instance="$hostname:9100",device=~"en.*"}[$__interval]))</t>
-  </si>
-  <si>
-    <t>Receive Current</t>
-  </si>
-  <si>
-    <t>sum(rate(node_network_receive_bytes_total{instance="hgx3b:9100",device=~"en.*"}[30s]))</t>
-  </si>
-  <si>
-    <t>Infiniband Throughput</t>
-  </si>
-  <si>
-    <t>sum(rate(node_infiniband_port_data_transmitted_bytes_total{instance="$hostname:9100"}[$__interval]))</t>
-  </si>
-  <si>
-    <t>sum(rate(node_infiniband_port_data_received_bytes_total{instance="$hostname:9100"}[$__interval]))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Network Traffic </t>
-  </si>
-  <si>
-    <t>irate(node_network_transmit_bytes_total{instance=\"$node\",job=\"$job\"}[$__rate_interval])*8</t>
-  </si>
-  <si>
-    <t>Network Traffic by Packets</t>
-  </si>
-  <si>
-    <t>Transmit</t>
-  </si>
-  <si>
-    <t>irate(node_network_transmit_packets_total{instance=\"$node\",job=\"$job\"}[$__rate_interval])</t>
-  </si>
-  <si>
-    <t>Receive</t>
-  </si>
-  <si>
-    <t>irate(node_network_receive_packets_total{instance=\"$node\",job=\"$job\"}[$__rate_interval])</t>
-  </si>
-  <si>
-    <t>Network Traffic Errors</t>
-  </si>
-  <si>
-    <t>irate(node_network_transmit_errs_total{instance=\"$node\",job=\"$job\"}[$__rate_interval])</t>
-  </si>
-  <si>
-    <t>irate(node_network_receive_errs_total{instance=\"$node\",job=\"$job\"}[$__rate_interval])</t>
-  </si>
-  <si>
     <t>Disk Metrics</t>
   </si>
   <si>
-    <t>Disk Usage</t>
-  </si>
-  <si>
-    <t>(sum(node_filesystem_size_bytes{device!="rootfs",instance="$hostname:9100"}) - sum(node_filesystem_avail_bytes{device!="rootfs",instance="$hostname:9100"})) / sum(node_filesystem_size_bytes{device!="rootfs",instance="$hostname:9100"})</t>
-  </si>
-  <si>
-    <t>Disk Throughput</t>
-  </si>
-  <si>
-    <t>sum by (instance) (rate(node_disk_io_time_ms{instance="$hostname:9100"}[$__interval]))</t>
-  </si>
-  <si>
-    <t>Disk IOps</t>
-  </si>
-  <si>
-    <t>irate(node_disk_writes_completed_total{instance=\"$node\",job=\"$job\",device=~\"$diskdevices\"}[$__rate_interval])</t>
-  </si>
-  <si>
-    <t>Disk R/W Data</t>
-  </si>
-  <si>
-    <t>irate(node_disk_written_bytes_total{instance=\"$node\",job=\"$job\"}[$__rate_interval])</t>
-  </si>
-  <si>
     <t>Metrics</t>
   </si>
   <si>
@@ -1528,6 +1384,26 @@
   </si>
   <si>
     <t>Difficult</t>
+  </si>
+  <si>
+    <t>avg(node_load1) by ( instance ) / count ( count (node_cpu_seconds_total) by (cpu, instance) ) by (instance) * 100</t>
+  </si>
+  <si>
+    <t>HeavyCpuLoad</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>Heavy CPU Load</t>
+  </si>
+  <si>
+    <t>avg(node_load1) by ( instance ) / count ( count (node_cpu_seconds_total) by (cpu, instance) ) by (instance) * 100&gt; 130
+avg(node_load1) by ( instance ) / count ( count (node_cpu_seconds_total) by (cpu, instance) ) by (instance) * 100 &gt; 200</t>
+  </si>
+  <si>
+    <t>Warning
+Critical</t>
   </si>
 </sst>
 </file>
@@ -1537,7 +1413,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1655,8 +1531,40 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1683,12 +1591,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1730,6 +1644,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="hair">
         <color auto="1"/>
       </left>
@@ -1739,8 +1679,21 @@
       <top style="hair">
         <color auto="1"/>
       </top>
-      <bottom style="hair">
-        <color auto="1"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1759,7 +1712,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1799,16 +1752,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1821,23 +1764,8 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1857,6 +1785,58 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Heading 1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -2452,26 +2432,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ36"/>
+  <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="53" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="74" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1"/>
     <col min="2" max="2" width="19.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.21875" style="2" customWidth="1"/>
     <col min="5" max="7" width="14.21875" style="2" customWidth="1"/>
     <col min="8" max="8" width="15.5546875" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.77734375" style="2" customWidth="1"/>
     <col min="10" max="10" width="13.21875" style="2" customWidth="1"/>
     <col min="11" max="11" width="100.44140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="25.21875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18" style="1" customWidth="1"/>
     <col min="13" max="13" width="29" style="1" customWidth="1"/>
     <col min="14" max="14" width="71.44140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="9.21875" style="4" customWidth="1"/>
@@ -2482,10 +2462,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -2541,7 +2521,7 @@
       <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="18" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="12"/>
@@ -2554,828 +2534,190 @@
       <c r="J2" s="12"/>
       <c r="K2" s="13"/>
       <c r="L2" s="14"/>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="19" t="s">
         <v>21</v>
       </c>
       <c r="O2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="P2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="Q2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="20" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="2" customFormat="1" ht="139.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="39">
         <v>100</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="39">
         <v>0</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="38">
         <v>0</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="39">
         <v>99</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="29" t="s">
+      <c r="M3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:18" s="46" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44">
+        <v>0</v>
+      </c>
+      <c r="G4" s="44">
+        <v>200</v>
+      </c>
+      <c r="H4" s="44">
+        <v>130</v>
+      </c>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="45" t="s">
+        <v>448</v>
+      </c>
+      <c r="L4" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19">
-        <v>100</v>
-      </c>
-      <c r="F4" s="19">
-        <v>0</v>
-      </c>
-      <c r="G4" s="19">
-        <v>95</v>
-      </c>
-      <c r="H4" s="19">
-        <v>85</v>
-      </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="30" t="s">
+      <c r="M4" s="42" t="s">
+        <v>449</v>
+      </c>
+      <c r="N4" s="42" t="s">
+        <v>452</v>
+      </c>
+      <c r="O4" s="42" t="s">
+        <v>450</v>
+      </c>
+      <c r="P4" s="42" t="s">
+        <v>453</v>
+      </c>
+      <c r="Q4" s="42" t="s">
+        <v>451</v>
+      </c>
+      <c r="R4" s="42" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="20"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="20"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="34"/>
+      <c r="O5" s="16"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="20"/>
-    </row>
-    <row r="8" spans="1:18" ht="55.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="20"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9" s="20"/>
-    </row>
-    <row r="10" spans="1:18" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19">
-        <v>100</v>
-      </c>
-      <c r="F10" s="19">
-        <v>0</v>
-      </c>
-      <c r="G10" s="19">
-        <v>90</v>
-      </c>
-      <c r="H10" s="19">
-        <v>80</v>
-      </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" s="20"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="20"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" s="20"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="L13" s="20"/>
-    </row>
-    <row r="14" spans="1:18" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="14"/>
-      <c r="O14" s="16"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="20"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="L16" s="20"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="20"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="L18" s="20"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="L19" s="20"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="20"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="L21" s="20"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="L22" s="20"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="L23" s="20"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="20"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="L25" s="20"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="L26" s="20"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="20"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="L28" s="20"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="L29" s="20"/>
-    </row>
-    <row r="30" spans="1:15" s="15" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="14"/>
-      <c r="O30" s="16"/>
-    </row>
-    <row r="31" spans="1:15" ht="42" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19">
-        <v>1</v>
-      </c>
-      <c r="F31" s="19">
-        <v>0</v>
-      </c>
-      <c r="G31" s="19">
-        <v>0.9</v>
-      </c>
-      <c r="H31" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="L31" s="20"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="L32" s="20"/>
-    </row>
-    <row r="33" spans="1:18" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="L33" s="20"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="L34" s="20"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="R36"/>
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -3407,263 +2749,263 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="119.21875" style="31" customWidth="1"/>
-    <col min="2" max="1024" width="11" style="31"/>
+    <col min="1" max="1" width="119.21875" style="22" customWidth="1"/>
+    <col min="2" max="1024" width="11" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:1" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="26" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="26" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="34" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="35" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="35" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="34" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="35" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="35" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="35" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="35" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="34" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="35" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="35" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="34" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="35" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="35" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="35" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="35" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="35" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="34" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="35" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="35" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="35" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="35" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3682,1722 +3024,1722 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.21875" style="36" customWidth="1"/>
-    <col min="2" max="2" width="45.5546875" style="36" customWidth="1"/>
-    <col min="3" max="1024" width="11" style="36"/>
+    <col min="1" max="1" width="56.21875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="45.5546875" style="27" customWidth="1"/>
+    <col min="3" max="1024" width="11" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="1:2" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="27" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="27" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="27" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="27" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="27" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="27" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="27" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="36" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="27" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="27" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="27" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="27" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="36" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="27" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="36" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="27" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="36" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="27" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="27" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="36" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="27" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="27" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="36" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="27" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="36" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="27" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="27" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="36" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="27" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="36" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="27" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="36" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="27" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="36" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="27" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="36" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="27" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="27" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="36" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="27" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="36" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="27" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="36" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="27" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="36" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="27" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="36" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="27" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="36" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="27" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="36" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="27" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="36" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="27" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="36" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="27" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="36" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="27" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="36" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="27" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="36" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="27" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="36" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="27" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="36" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="27" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="36" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="27" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="36" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="27" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="36" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="27" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="36" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" s="27" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="36" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="27" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="36" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="27" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="36" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="27" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="36" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="27" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="36" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="27" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="36" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" s="27" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="36" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="27" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="36" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="27" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="36" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="27" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="36" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="27" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="36" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="27" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="36" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="27" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="36" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="27" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="36" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="27" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="36" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="27" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="36" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="27" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="36" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" s="27" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="36" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" s="27" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="36" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" s="27" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="36" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" s="27" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="36" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" s="27" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="36" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="27" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="36" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="27" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="36" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="27" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="36" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="27" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="36" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" s="27" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="36" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" s="27" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="36" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="27" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="36" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" s="27" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="36" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" s="27" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="36" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="27" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="36" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" s="27" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="36" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" s="27" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="36" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="27" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="36" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="27" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="36" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" s="27" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="36" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="27" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="36" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="27" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="36" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" s="27" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="36" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="27" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="36" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" s="27" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="36" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" s="27" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="36" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" s="27" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="36" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" s="27" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="36" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" s="27" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="36" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" s="27" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="36" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" s="27" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="36" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" s="27" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="36" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" s="27" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="36" t="s">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" s="27" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="36" t="s">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" s="27" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="36" t="s">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" s="27" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="36" t="s">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" s="27" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="36" t="s">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" s="27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="36" t="s">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" s="27" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="36" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" s="27" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="36" t="s">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" s="27" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="36" t="s">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" s="27" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="36" t="s">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" s="27" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="36" t="s">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" s="27" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="36" t="s">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" s="27" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="36" t="s">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" s="27" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="36" t="s">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" s="27" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="36" t="s">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" s="27" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" s="36" t="s">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" s="27" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="36" t="s">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" s="27" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="36" t="s">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" s="27" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="36" t="s">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" s="27" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="36" t="s">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" s="27" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="36" t="s">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" s="27" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" s="36" t="s">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" s="27" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" s="36" t="s">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" s="27" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" s="36" t="s">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" s="27" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="36" t="s">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" s="27" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" s="36" t="s">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" s="27" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" s="36" t="s">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" s="27" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" s="36" t="s">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" s="27" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" s="36" t="s">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" s="27" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" s="36" t="s">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" s="27" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" s="36" t="s">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" s="27" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" s="36" t="s">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" s="27" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" s="36" t="s">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" s="27" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" s="36" t="s">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" s="27" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" s="36" t="s">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" s="27" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" s="36" t="s">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" s="27" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="36" t="s">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" s="27" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="36" t="s">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" s="27" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" s="36" t="s">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" s="27" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" s="36" t="s">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181" s="27" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" s="36" t="s">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182" s="27" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135" s="36" t="s">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183" s="27" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" s="36" t="s">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184" s="27" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" s="36" t="s">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185" s="27" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138" s="36" t="s">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186" s="27" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" s="36" t="s">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187" s="27" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" s="36" t="s">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188" s="27" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141" s="36" t="s">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" s="27" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142" s="36" t="s">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190" s="27" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143" s="36" t="s">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191" s="27" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144" s="36" t="s">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192" s="27" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145" s="36" t="s">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" s="27" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146" s="36" t="s">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194" s="27" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147" s="36" t="s">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195" s="27" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" s="36" t="s">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" s="27" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149" s="36" t="s">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197" s="27" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150" s="36" t="s">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198" s="27" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" s="36" t="s">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199" s="27" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152" s="36" t="s">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200" s="27" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153" s="36" t="s">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201" s="27" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154" s="36" t="s">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202" s="27" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155" s="36" t="s">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A203" s="27" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156" s="36" t="s">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204" s="27" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157" s="36" t="s">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A205" s="27" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158" s="36" t="s">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206" s="27" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A159" s="36" t="s">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A207" s="27" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160" s="36" t="s">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208" s="27" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A161" s="36" t="s">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209" s="27" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A162" s="36" t="s">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210" s="27" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A163" s="36" t="s">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211" s="27" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A164" s="36" t="s">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212" s="27" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A165" s="36" t="s">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A166" s="36" t="s">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A214" s="27" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A167" s="36" t="s">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215" s="27" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A168" s="36" t="s">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A216" s="27" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A169" s="36" t="s">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217" s="27" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A170" s="36" t="s">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218" s="27" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A171" s="36" t="s">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A219" s="27" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A172" s="36" t="s">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A220" s="27" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A173" s="36" t="s">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A221" s="27" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A174" s="36" t="s">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222" s="27" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A175" s="36" t="s">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A223" s="27" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A176" s="36" t="s">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224" s="27" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177" s="36" t="s">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225" s="27" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A178" s="36" t="s">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226" s="27" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A179" s="36" t="s">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227" s="27" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A180" s="36" t="s">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228" s="27" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A181" s="36" t="s">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229" s="27" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A182" s="36" t="s">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230" s="27" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A183" s="36" t="s">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231" s="27" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A184" s="36" t="s">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232" s="27" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A185" s="36" t="s">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233" s="27" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A186" s="36" t="s">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234" s="27" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A187" s="36" t="s">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235" s="27" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A188" s="36" t="s">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236" s="27" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A189" s="36" t="s">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A237" s="27" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A190" s="36" t="s">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238" s="27" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A191" s="36" t="s">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239" s="27" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A192" s="36" t="s">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240" s="27" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A193" s="36" t="s">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241" s="27" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A194" s="36" t="s">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A242" s="27" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A195" s="36" t="s">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243" s="27" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A196" s="36" t="s">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244" s="27" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A197" s="36" t="s">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245" s="27" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A198" s="36" t="s">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246" s="27" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A199" s="36" t="s">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247" s="27" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A200" s="36" t="s">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248" s="27" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A201" s="36" t="s">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249" s="27" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A202" s="36" t="s">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250" s="27" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A203" s="36" t="s">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251" s="27" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A204" s="36" t="s">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252" s="27" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A205" s="36" t="s">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253" s="27" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A206" s="36" t="s">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254" s="27" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A207" s="36" t="s">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255" s="27" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A208" s="36" t="s">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A256" s="27" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A209" s="36" t="s">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A257" s="27" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A210" s="36" t="s">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A258" s="27" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A211" s="36" t="s">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259" s="27" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A212" s="36" t="s">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A260" s="27" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A213" s="36" t="s">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A261" s="27" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A214" s="36" t="s">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A262" s="27" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A215" s="36" t="s">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A263" s="27" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A216" s="36" t="s">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A264" s="27" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A217" s="36" t="s">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A265" s="27" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A218" s="36" t="s">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A266" s="27" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A219" s="36" t="s">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A267" s="27" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A220" s="36" t="s">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A268" s="27" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A221" s="36" t="s">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A269" s="27" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A222" s="36" t="s">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A270" s="27" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A223" s="36" t="s">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A271" s="27" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A224" s="36" t="s">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A272" s="27" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A225" s="36" t="s">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A273" s="27" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A226" s="36" t="s">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A274" s="27" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A227" s="36" t="s">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A275" s="27" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A228" s="36" t="s">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276" s="27" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A229" s="36" t="s">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A277" s="27" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A230" s="36" t="s">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A278" s="27" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A231" s="36" t="s">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279" s="27" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A232" s="36" t="s">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A280" s="27" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A233" s="36" t="s">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A281" s="27" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A234" s="36" t="s">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282" s="27" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A235" s="36" t="s">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A283" s="27" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A236" s="36" t="s">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A284" s="27" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A237" s="36" t="s">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A285" s="27" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A238" s="36" t="s">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A286" s="27" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A239" s="36" t="s">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A287" s="27" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A240" s="36" t="s">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A288" s="27" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A241" s="36" t="s">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A289" s="27" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A242" s="36" t="s">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A290" s="27" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A243" s="36" t="s">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A291" s="27" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A244" s="36" t="s">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A292" s="27" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A245" s="36" t="s">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A293" s="27" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A246" s="36" t="s">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A294" s="27" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A247" s="36" t="s">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A295" s="27" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A248" s="36" t="s">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A296" s="27" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A249" s="36" t="s">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A297" s="27" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A250" s="36" t="s">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A298" s="27" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A251" s="36" t="s">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299" s="27" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A252" s="36" t="s">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A300" s="27" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A253" s="36" t="s">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A301" s="27" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A254" s="36" t="s">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A302" s="27" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A255" s="36" t="s">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303" s="27" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A256" s="36" t="s">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304" s="27" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A257" s="36" t="s">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305" s="27" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A258" s="36" t="s">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306" s="27" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A259" s="36" t="s">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307" s="27" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A260" s="36" t="s">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308" s="27" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A261" s="36" t="s">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309" s="27" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A262" s="36" t="s">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310" s="27" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A263" s="36" t="s">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A311" s="27" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A264" s="36" t="s">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A312" s="27" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A265" s="36" t="s">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A313" s="27" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A266" s="36" t="s">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314" s="27" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A267" s="36" t="s">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315" s="27" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A268" s="36" t="s">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A316" s="27" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A269" s="36" t="s">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A317" s="27" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A270" s="36" t="s">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A318" s="27" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A271" s="36" t="s">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A319" s="27" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A272" s="36" t="s">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A320" s="27" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A273" s="36" t="s">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A321" s="27" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A274" s="36" t="s">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A322" s="27" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A275" s="36" t="s">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A323" s="27" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A276" s="36" t="s">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A324" s="27" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A277" s="36" t="s">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A325" s="27" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A278" s="36" t="s">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A326" s="27" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A279" s="36" t="s">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A327" s="27" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A280" s="36" t="s">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A328" s="27" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A281" s="36" t="s">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A329" s="27" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A282" s="36" t="s">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A330" s="27" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A283" s="36" t="s">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A331" s="27" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A284" s="36" t="s">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A332" s="27" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A285" s="36" t="s">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A333" s="27" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A286" s="36" t="s">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A334" s="27" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A287" s="36" t="s">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A335" s="27" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A288" s="36" t="s">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A336" s="27" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A289" s="36" t="s">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A337" s="27" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A290" s="36" t="s">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A338" s="27" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A291" s="36" t="s">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A339" s="27" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A292" s="36" t="s">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A340" s="27" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A293" s="36" t="s">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A341" s="27" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A294" s="36" t="s">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A342" s="27" t="s">
         <v>428</v>
-      </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A295" s="36" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A296" s="36" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A297" s="36" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A298" s="36" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A299" s="36" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A300" s="36" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A301" s="36" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A302" s="36" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A303" s="36" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A304" s="36" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A305" s="36" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A306" s="36" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A307" s="36" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A308" s="36" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A309" s="36" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A310" s="36" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A311" s="36" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A312" s="36" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A313" s="36" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A314" s="36" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A315" s="36" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A316" s="36" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A317" s="36" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A318" s="36" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A319" s="36" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A320" s="36" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A321" s="36" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A322" s="36" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A323" s="36" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A324" s="36" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A325" s="36" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A326" s="36" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A327" s="36" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A328" s="36" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A329" s="36" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A330" s="36" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A331" s="36" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A332" s="36" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A333" s="36" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A334" s="36" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A335" s="36" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A336" s="36" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A337" s="36" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A338" s="36" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A339" s="36" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A340" s="36" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A341" s="36" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A342" s="36" t="s">
-        <v>476</v>
       </c>
     </row>
   </sheetData>
@@ -5416,153 +4758,153 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.21875" style="31" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" style="31" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="31" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" style="31" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" style="31" customWidth="1"/>
-    <col min="6" max="6" width="28" style="31" customWidth="1"/>
-    <col min="7" max="1024" width="11" style="31"/>
+    <col min="1" max="1" width="31.21875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" style="22" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="27.77734375" style="22" customWidth="1"/>
+    <col min="6" max="6" width="28" style="22" customWidth="1"/>
+    <col min="7" max="1024" width="11" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="33" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>477</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>478</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>480</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>481</v>
+    <row r="1" spans="1:6" s="24" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>429</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>430</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>431</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>432</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
-        <v>482</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>483</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>483</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>483</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>484</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>485</v>
+      <c r="A2" s="29" t="s">
+        <v>434</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
-        <v>486</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>487</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>487</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>488</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>490</v>
+      <c r="A3" s="29" t="s">
+        <v>438</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
-        <v>491</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>487</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>487</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>483</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>490</v>
+      <c r="A4" s="29" t="s">
+        <v>443</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="38" t="s">
-        <v>492</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>490</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>490</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>487</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>484</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>490</v>
+      <c r="A5" s="29" t="s">
+        <v>444</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
-        <v>493</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>483</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>487</v>
-      </c>
-      <c r="D6" s="38" t="s">
-        <v>483</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>485</v>
+      <c r="A6" s="29" t="s">
+        <v>445</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
-        <v>494</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>490</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>490</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>483</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="F7" s="38" t="s">
-        <v>495</v>
+      <c r="A7" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>441</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>